<commit_message>
vMX VMs cloning from templates
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="vm_template_pb.yml" sheetId="1" r:id="rId1"/>
+    <sheet name="vm_deployment_pb.yml" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
   <si>
     <t>ovftool_path:</t>
   </si>
@@ -146,9 +147,6 @@
     <t>/usr/bin/</t>
   </si>
   <si>
-    <t>10.33.94.16</t>
-  </si>
-  <si>
     <t>TFI-LAB</t>
   </si>
   <si>
@@ -168,9 +166,6 @@
   </si>
   <si>
     <t>vuser:</t>
-  </si>
-  <si>
-    <t>admin</t>
   </si>
   <si>
     <t>vpassword:</t>
@@ -264,12 +259,125 @@
   <si>
     <t>vm-to-template.yml</t>
   </si>
+  <si>
+    <t>10.33.95.200</t>
+  </si>
+  <si>
+    <t>administrator@vsphere.local</t>
+  </si>
+  <si>
+    <t>group_vars/all/vars.yml</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10.33.94.180</t>
+  </si>
+  <si>
+    <t>group_vars/vmxlab/vars.yml</t>
+  </si>
+  <si>
+    <t>rpool:</t>
+  </si>
+  <si>
+    <t>vmwarehost:</t>
+  </si>
+  <si>
+    <t>"/Resources/net"</t>
+  </si>
+  <si>
+    <t>"Laboratory\\LAB\ Cluster\ 2"</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>vmx-vm-clone.yml</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> False</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "{{ vcenter }}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "{{ vuser }}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "{{ vpassword }}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "{{ cluster }}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "{{ rpool }}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "{{ datacenter }}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "{{ vmwarehost }}"</t>
+  </si>
+  <si>
+    <t>vm_create_pb.yml</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>17.2R1.13 17.1R1.8 16.2R1.6, 16.1R2.11, 16.1R1.7, 15.1F6.9 [17.2R1.13]</t>
+  </si>
+  <si>
+    <t>vmx_vmware_lab/mylab/hosts</t>
+  </si>
+  <si>
+    <t>{{ inventory_hostname }}</t>
+  </si>
+  <si>
+    <t>vmxlab</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "{{ inventory_hostname }}_vfpc_{{ version }}"
+"vMX_vfpc_{{ version }}"</t>
+  </si>
+  <si>
+    <t>datacenter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vcenter_hostname</t>
+  </si>
+  <si>
+    <t>cluster</t>
+  </si>
+  <si>
+    <t>validate_certs</t>
+  </si>
+  <si>
+    <t>resource_pool</t>
+  </si>
+  <si>
+    <t>hostname</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>guest
+template_src</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,8 +403,17 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,8 +438,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -499,11 +622,318 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -523,9 +953,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -544,14 +971,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -559,23 +989,146 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -856,16 +1409,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
@@ -876,233 +1429,239 @@
     <col min="11" max="11" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="33"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="12" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="13"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="28"/>
+      <c r="J1" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>38</v>
+      <c r="A2" s="32" t="s">
+        <v>76</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>39</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="15" t="s">
         <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="32"/>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>2</v>
+      <c r="D3" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="14" t="s">
+        <v>8</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="14"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="15"/>
+      <c r="H5" s="14"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="15"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="32"/>
+      <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="14"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="15"/>
+      <c r="H6" s="14"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="15"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="15"/>
+      <c r="H7" s="14"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="15"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="16" t="s">
-        <v>46</v>
+      <c r="A8" s="34"/>
+      <c r="B8" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="C8" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="16"/>
+      <c r="H8" s="15"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="16"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="17"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="17"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="17"/>
+      <c r="F9" s="16"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="17"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="17"/>
+      <c r="J9" s="16"/>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="B10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>69</v>
+      <c r="H10" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="J10" s="17" t="s">
         <v>4</v>
       </c>
       <c r="K10" s="4" t="s">
@@ -1111,31 +1670,31 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>70</v>
+      <c r="H11" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="18" t="s">
         <v>6</v>
       </c>
       <c r="K11" s="5" t="s">
@@ -1144,67 +1703,67 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="17"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="17"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="17"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="17"/>
+      <c r="H12" s="16"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="17"/>
+      <c r="J12" s="16"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>52</v>
+      <c r="A13" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="20"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="20"/>
+      <c r="H13" s="19"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="20"/>
+      <c r="J13" s="19"/>
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="21" t="s">
-        <v>54</v>
+      <c r="A14" s="36"/>
+      <c r="B14" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="21" t="s">
-        <v>71</v>
+      <c r="H14" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="20" t="s">
         <v>18</v>
       </c>
       <c r="K14" s="10" t="s">
@@ -1212,144 +1771,514 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="21" t="s">
-        <v>56</v>
+      <c r="A15" s="36"/>
+      <c r="B15" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>20</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="21"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="21"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="21"/>
+      <c r="J15" s="20"/>
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="21" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="20" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="21"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="21"/>
+      <c r="H16" s="20"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="21"/>
+      <c r="J16" s="20"/>
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="21" t="s">
-        <v>58</v>
+      <c r="A17" s="36"/>
+      <c r="B17" s="20" t="s">
+        <v>56</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>24</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="21"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="21"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="21"/>
+      <c r="J17" s="20"/>
       <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="21" t="s">
+      <c r="A18" s="36"/>
+      <c r="B18" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>26</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="21"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="21"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="21"/>
+      <c r="J18" s="20"/>
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="36"/>
+      <c r="B19" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="1:11" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="22"/>
+      <c r="C20" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="21"/>
       <c r="E20" s="11"/>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="J20" s="22"/>
+      <c r="H20" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="J20" s="21"/>
       <c r="K20" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A4:A8"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A2:A3"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="49" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="66" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="80"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="86" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34"/>
+      <c r="B3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="82" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="83" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="84"/>
+      <c r="E4" s="85"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="73"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="73"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="38"/>
+      <c r="B8" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="52" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="88" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="86" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="45"/>
+      <c r="B10" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="73"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="46"/>
+      <c r="B11" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="87" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="90"/>
+      <c r="J12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30"/>
+      <c r="B14" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="78" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="47"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="75"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="74"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="74"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="74"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="74"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="36"/>
+      <c r="B21" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="74"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
+      <c r="B22" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="74"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="76"/>
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="47"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="69"/>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="70" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="60" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="91" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="61"/>
+      <c r="E26" s="62"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C13" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
variable version added to vm_template_pb.yml
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="vm_template_pb.yml" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="120">
   <si>
     <t>ovftool_path:</t>
   </si>
@@ -112,12 +112,6 @@
   </si>
   <si>
     <t>ssl_verify:</t>
-  </si>
-  <si>
-    <t>ovftool.yml</t>
-  </si>
-  <si>
-    <t>vm-add-nic.yml</t>
   </si>
   <si>
     <t>vcenter_ip:</t>
@@ -228,9 +222,6 @@
     <t>CP / FPC</t>
   </si>
   <si>
-    <t>vm-config.ym</t>
-  </si>
-  <si>
     <t>vcenter_hostname:</t>
   </si>
   <si>
@@ -257,9 +248,6 @@
     <t>{{ datacenter }}</t>
   </si>
   <si>
-    <t>vm-to-template.yml</t>
-  </si>
-  <si>
     <t>10.33.95.200</t>
   </si>
   <si>
@@ -320,13 +308,7 @@
     <t xml:space="preserve"> "{{ vmwarehost }}"</t>
   </si>
   <si>
-    <t>vm_create_pb.yml</t>
-  </si>
-  <si>
     <t>version</t>
-  </si>
-  <si>
-    <t>17.2R1.13 17.1R1.8 16.2R1.6, 16.1R2.11, 16.1R1.7, 15.1F6.9 [17.2R1.13]</t>
   </si>
   <si>
     <t>vmx_vmware_lab/mylab/hosts</t>
@@ -371,6 +353,51 @@
   <si>
     <t>guest
 template_src</t>
+  </si>
+  <si>
+    <t>vm_deployment_pb.yml</t>
+  </si>
+  <si>
+    <t>[17.4R1.16] 17.2R1.13 17.1R1.8 16.2R1.6, 16.1R2.11, 16.1R1.7</t>
+  </si>
+  <si>
+    <t>vm_template_pb.yml</t>
+  </si>
+  <si>
+    <t>"vfpc_{{ version }}.ova"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vmname: </t>
+  </si>
+  <si>
+    <t>vMX_vfpc_{{ version }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ovafile: </t>
+  </si>
+  <si>
+    <t>vCP.yml (host_vars)</t>
+  </si>
+  <si>
+    <t>"vcp_{{ version }}.ova"</t>
+  </si>
+  <si>
+    <t>vMX_vcp_{{ version }}</t>
+  </si>
+  <si>
+    <t>vFPC.yml (host_vars)</t>
+  </si>
+  <si>
+    <t>ovftool.yml (tasks)</t>
+  </si>
+  <si>
+    <t>vm-add-nic.yml (tasks)</t>
+  </si>
+  <si>
+    <t>vm-config.ym (tasks)</t>
+  </si>
+  <si>
+    <t>vm-to-template.yml (tasks)</t>
   </si>
 </sst>
 </file>
@@ -445,7 +472,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -926,6 +953,41 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -933,7 +995,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -971,44 +1033,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1016,15 +1048,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1043,15 +1066,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1095,15 +1109,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1124,6 +1129,115 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1407,11 +1521,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,41 +1543,53 @@
     <col min="9" max="9" width="18.42578125" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+    <col min="15" max="15" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="28"/>
-      <c r="F1" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="28"/>
-      <c r="J1" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="28"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="76"/>
+      <c r="F1" s="75" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="76"/>
+      <c r="H1" s="75" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="76"/>
+      <c r="J1" s="75" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="96"/>
+      <c r="L1" s="114" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" s="115"/>
+      <c r="N1" s="114" t="s">
+        <v>112</v>
+      </c>
+      <c r="O1" s="115"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="78" t="s">
+        <v>72</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>2</v>
@@ -1470,31 +1598,35 @@
         <v>3</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
+        <v>29</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="100"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="78"/>
       <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>8</v>
@@ -1508,20 +1640,24 @@
         <v>8</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J3" s="14"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
-        <v>38</v>
+      <c r="K3" s="37"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="7"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="77" t="s">
+        <v>36</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>0</v>
@@ -1534,15 +1670,19 @@
       <c r="H4" s="13"/>
       <c r="I4" s="6"/>
       <c r="J4" s="13"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="101"/>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="78"/>
       <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>10</v>
@@ -1555,15 +1695,19 @@
       <c r="H5" s="14"/>
       <c r="I5" s="7"/>
       <c r="J5" s="14"/>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="100"/>
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="78"/>
       <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>12</v>
@@ -1576,15 +1720,19 @@
       <c r="H6" s="14"/>
       <c r="I6" s="7"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="100"/>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="78"/>
       <c r="B7" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>14</v>
@@ -1597,12 +1745,16 @@
       <c r="H7" s="14"/>
       <c r="I7" s="7"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="34"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="79"/>
       <c r="B8" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="8" t="b">
         <v>0</v>
@@ -1618,9 +1770,13 @@
       <c r="H8" s="15"/>
       <c r="I8" s="8"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="40"/>
+      <c r="L8" s="102"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="102"/>
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="16"/>
       <c r="C9" s="3"/>
@@ -1631,17 +1787,21 @@
       <c r="H9" s="16"/>
       <c r="I9" s="3"/>
       <c r="J9" s="16"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>48</v>
+      <c r="K9" s="35"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="80" t="s">
+        <v>46</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>75</v>
+        <v>44</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>71</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>4</v>
@@ -1653,28 +1813,32 @@
         <v>4</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J10" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
+      <c r="K10" s="97" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="103"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="103"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="81"/>
       <c r="B11" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>6</v>
@@ -1686,22 +1850,26 @@
         <v>6</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="104"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="104"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="16"/>
       <c r="C12" s="3"/>
@@ -1712,17 +1880,21 @@
       <c r="H12" s="16"/>
       <c r="I12" s="3"/>
       <c r="J12" s="16"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>63</v>
+      <c r="K12" s="35"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="73" t="s">
+        <v>61</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>16</v>
@@ -1735,15 +1907,19 @@
       <c r="H13" s="19"/>
       <c r="I13" s="9"/>
       <c r="J13" s="19"/>
-      <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="105"/>
+      <c r="O13" s="9"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="74"/>
       <c r="B14" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>18</v>
@@ -1755,28 +1931,32 @@
         <v>18</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
+      <c r="K14" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="106"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="106"/>
+      <c r="O14" s="10"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="74"/>
       <c r="B15" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>20</v>
@@ -1789,15 +1969,19 @@
       <c r="H15" s="20"/>
       <c r="I15" s="10"/>
       <c r="J15" s="20"/>
-      <c r="K15" s="10"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="106"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="106"/>
+      <c r="O15" s="10"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="74"/>
       <c r="B16" s="20" t="s">
         <v>22</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>22</v>
@@ -1810,15 +1994,19 @@
       <c r="H16" s="20"/>
       <c r="I16" s="10"/>
       <c r="J16" s="20"/>
-      <c r="K16" s="10"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="106"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="106"/>
+      <c r="O16" s="10"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="74"/>
       <c r="B17" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>24</v>
@@ -1831,15 +2019,19 @@
       <c r="H17" s="20"/>
       <c r="I17" s="10"/>
       <c r="J17" s="20"/>
-      <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="106"/>
+      <c r="O17" s="10"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="74"/>
       <c r="B18" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>26</v>
@@ -1852,15 +2044,19 @@
       <c r="H18" s="20"/>
       <c r="I18" s="10"/>
       <c r="J18" s="20"/>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="106"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="106"/>
+      <c r="O18" s="10"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="74"/>
       <c r="B19" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="10"/>
@@ -1869,37 +2065,107 @@
       <c r="H19" s="20"/>
       <c r="I19" s="10"/>
       <c r="J19" s="20"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37" t="s">
-        <v>62</v>
+      <c r="K19" s="44"/>
+      <c r="L19" s="106"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="106"/>
+      <c r="O19" s="10"/>
+    </row>
+    <row r="20" spans="1:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28" t="s">
+        <v>60</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="11"/>
       <c r="F20" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J20" s="21"/>
-      <c r="K20" s="11"/>
+      <c r="K20" s="98"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="107"/>
+      <c r="O20" s="11"/>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="112" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="94" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="95"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="95"/>
+      <c r="I22" s="95"/>
+      <c r="J22" s="95"/>
+      <c r="K22" s="95"/>
+      <c r="L22" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="M22" s="108" t="s">
+        <v>108</v>
+      </c>
+      <c r="N22" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="O22" s="108" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="113"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="110"/>
+      <c r="D23" s="111"/>
+      <c r="E23" s="111"/>
+      <c r="F23" s="111"/>
+      <c r="G23" s="111"/>
+      <c r="H23" s="111"/>
+      <c r="I23" s="111"/>
+      <c r="J23" s="111"/>
+      <c r="K23" s="111"/>
+      <c r="L23" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="M23" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="N23" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="O23" s="46" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="13">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A4:A8"/>
@@ -1921,9 +2187,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,338 +2197,338 @@
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="49" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="36" customWidth="1"/>
     <col min="5" max="5" width="43.7109375" customWidth="1"/>
     <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="66" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="50" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="79" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="80"/>
+        <v>79</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="82" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="83"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>76</v>
+      <c r="A2" s="77" t="s">
+        <v>72</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="86" t="s">
-        <v>103</v>
+      <c r="C2" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>97</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34"/>
+      <c r="A3" s="79"/>
       <c r="B3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="87" t="s">
-        <v>102</v>
+      <c r="C3" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>96</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="82" t="s">
+      <c r="A4" s="88" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="83" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="84"/>
-      <c r="E4" s="85"/>
+      <c r="C4" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="65"/>
+      <c r="E4" s="66"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="78"/>
       <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="73" t="s">
-        <v>104</v>
+      <c r="C5" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>98</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="A6" s="78"/>
       <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="57"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="78"/>
+      <c r="B7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="73"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="14" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="89"/>
+      <c r="B8" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="73"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="52" t="b">
+      <c r="C8" s="39" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="88" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>86</v>
+      <c r="D8" s="69" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="67" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="91"/>
+      <c r="B10" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="86" t="s">
-        <v>106</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="73"/>
+      <c r="D10" s="57"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
-      <c r="B11" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="87" t="s">
-        <v>107</v>
+      <c r="A11" s="92"/>
+      <c r="B11" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>101</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="90"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="71"/>
       <c r="J12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="80" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="81"/>
+      <c r="B14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="35" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="34"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30"/>
-      <c r="B14" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="55" t="s">
+      <c r="C16" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="78" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="19" t="s">
+      <c r="D16" s="59"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="74"/>
+      <c r="B17" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C17" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="75"/>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="20" t="s">
+      <c r="D17" s="58"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="74"/>
+      <c r="B18" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C18" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="74"/>
+      <c r="D18" s="58"/>
       <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="36"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="74"/>
+      <c r="C19" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="58"/>
       <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="36"/>
+      <c r="A20" s="74"/>
       <c r="B20" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="74"/>
+        <v>54</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="58"/>
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="58"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="74"/>
+      <c r="B22" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="58"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="74"/>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
-      <c r="B22" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" ht="104.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="76"/>
+      <c r="D23" s="60"/>
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="47"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="69"/>
-    </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="64" t="s">
+      <c r="A24" s="34"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="53"/>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="84" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="70" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="E25" s="60" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="91" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" s="65" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="62"/>
+      <c r="A26" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="85"/>
+      <c r="E26" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>